<commit_message>
Excel changes for common Pages class
</commit_message>
<xml_diff>
--- a/src/test/resources/ExcelFiles/AssessmentCenterDetails.xlsx
+++ b/src/test/resources/ExcelFiles/AssessmentCenterDetails.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28324"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://focalpointk12-my.sharepoint.com/personal/gopi_pagadala_focalpointk12_com/Documents/FPK12 Automation-2024/FPK12-AssessmentCenter/src/test/resources/ExcelFiles/"/>
     </mc:Choice>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="53">
   <si>
     <t>FirstName</t>
   </si>
@@ -138,12 +138,55 @@
   </si>
   <si>
     <t>46461</t>
+  </si>
+  <si>
+    <t>FPK12School24523</t>
+  </si>
+  <si>
+    <t>47523</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>95638</t>
+  </si>
+  <si>
+    <t>48045</t>
+  </si>
+  <si>
+    <t>FPK12School93651</t>
+  </si>
+  <si>
+    <t>FPK12Classroom85010</t>
+  </si>
+  <si>
+    <t>FPK12Section79808</t>
+  </si>
+  <si>
+    <t>40477</t>
+  </si>
+  <si>
+    <t>56244</t>
+  </si>
+  <si>
+    <t>53805</t>
+  </si>
+  <si>
+    <t>FPK12School56333</t>
+  </si>
+  <si>
+    <t>FPK12Classroom30485</t>
+  </si>
+  <si>
+    <t>FPK12Section88289</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -212,7 +255,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -257,12 +300,19 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <right style="thin"/>
+      <bottom style="thin"/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -319,6 +369,33 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -633,21 +710,21 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="30" customWidth="1"/>
-    <col min="2" max="2" width="23.5546875" customWidth="1"/>
-    <col min="3" max="3" width="24.77734375" customWidth="1"/>
-    <col min="4" max="4" width="19.88671875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="23.77734375" style="1" customWidth="1"/>
-    <col min="7" max="7" width="20.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="31.5546875" customWidth="1"/>
-    <col min="10" max="10" width="19.77734375" customWidth="1"/>
-    <col min="11" max="11" width="15" customWidth="1"/>
-    <col min="12" max="12" width="18.33203125" customWidth="1"/>
-    <col min="13" max="13" width="19.33203125" customWidth="1"/>
-    <col min="14" max="14" width="23.6640625" customWidth="1"/>
-    <col min="15" max="15" width="20.109375" customWidth="1"/>
-    <col min="16" max="16" width="16.109375" customWidth="1"/>
-    <col min="17" max="17" width="15" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="30.0"/>
+    <col min="2" max="2" customWidth="true" width="23.5546875"/>
+    <col min="3" max="3" customWidth="true" width="24.77734375"/>
+    <col min="4" max="4" customWidth="true" style="1" width="19.88671875"/>
+    <col min="5" max="5" customWidth="true" style="1" width="23.77734375"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" style="1" width="20.5546875"/>
+    <col min="8" max="8" customWidth="true" width="31.5546875"/>
+    <col min="10" max="10" customWidth="true" width="19.77734375"/>
+    <col min="11" max="11" customWidth="true" width="15.0"/>
+    <col min="12" max="12" customWidth="true" width="18.33203125"/>
+    <col min="13" max="13" customWidth="true" width="19.33203125"/>
+    <col min="14" max="14" customWidth="true" width="23.6640625"/>
+    <col min="15" max="15" customWidth="true" width="20.109375"/>
+    <col min="16" max="16" customWidth="true" width="16.109375"/>
+    <col min="17" max="17" customWidth="true" width="15.0"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.3">
@@ -692,14 +769,14 @@
       <c r="O1" s="10"/>
     </row>
     <row r="2" spans="1:18" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="B2" s="20" t="s">
-        <v>33</v>
-      </c>
-      <c r="C2" s="20" t="s">
-        <v>34</v>
+      <c r="A2" t="s" s="27">
+        <v>50</v>
+      </c>
+      <c r="B2" t="s" s="28">
+        <v>51</v>
+      </c>
+      <c r="C2" t="s" s="29">
+        <v>52</v>
       </c>
       <c r="D2" s="13" t="s">
         <v>9</v>
@@ -743,7 +820,7 @@
         <v>13</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>36</v>
+        <v>47</v>
       </c>
       <c r="F3" s="13">
         <v>1323</v>
@@ -765,7 +842,7 @@
         <v>14</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>37</v>
+        <v>48</v>
       </c>
       <c r="F4" s="13">
         <v>1323</v>
@@ -787,7 +864,7 @@
         <v>15</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>38</v>
+        <v>49</v>
       </c>
       <c r="F5" s="13">
         <v>1323</v>
@@ -831,16 +908,16 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="30" customWidth="1"/>
-    <col min="2" max="2" width="20" customWidth="1"/>
-    <col min="3" max="3" width="16" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.88671875" style="10" customWidth="1"/>
-    <col min="5" max="5" width="23.77734375" style="1" customWidth="1"/>
-    <col min="7" max="7" width="11.5546875" customWidth="1"/>
-    <col min="8" max="8" width="38.44140625" style="1" customWidth="1"/>
-    <col min="11" max="11" width="14.21875" customWidth="1"/>
-    <col min="12" max="12" width="15" customWidth="1"/>
-    <col min="13" max="13" width="18.33203125" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="30.0"/>
+    <col min="2" max="2" customWidth="true" width="20.0"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="16.0"/>
+    <col min="4" max="4" customWidth="true" style="10" width="19.88671875"/>
+    <col min="5" max="5" customWidth="true" style="1" width="23.77734375"/>
+    <col min="7" max="7" customWidth="true" width="11.5546875"/>
+    <col min="8" max="8" customWidth="true" style="1" width="38.44140625"/>
+    <col min="11" max="11" customWidth="true" width="14.21875"/>
+    <col min="12" max="12" customWidth="true" width="15.0"/>
+    <col min="13" max="13" customWidth="true" width="18.33203125"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Attached Downloaded file to Extent report
</commit_message>
<xml_diff>
--- a/src/test/resources/ExcelFiles/AssessmentCenterDetails.xlsx
+++ b/src/test/resources/ExcelFiles/AssessmentCenterDetails.xlsx
@@ -3,14 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28324"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://focalpointk12-my.sharepoint.com/personal/gopi_pagadala_focalpointk12_com/Documents/FPK12 Automation-2024/FPK12-AssessmentCenter/src/test/resources/ExcelFiles/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="18" documentId="13_ncr:1_{0F536124-3BAA-43E7-ADC9-936F10A8E639}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6D1A48D8-CF0D-4FD3-8906-FC140A439001}"/>
+  <xr:revisionPtr revIDLastSave="27" documentId="13_ncr:1_{0F536124-3BAA-43E7-ADC9-936F10A8E639}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{173A4F2A-FC2F-445C-805C-D994E52DF10C}"/>
   <bookViews>
-    <workbookView xWindow="1536" yWindow="1536" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1116" yWindow="1116" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="STAGE" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="39">
   <si>
     <t>FirstName</t>
   </si>
@@ -50,143 +50,100 @@
     <t>Year</t>
   </si>
   <si>
+    <t>@Abcd1234</t>
+  </si>
+  <si>
+    <t>password</t>
+  </si>
+  <si>
+    <t>fpk12admin</t>
+  </si>
+  <si>
+    <t>fpk12teacher</t>
+  </si>
+  <si>
+    <t>fpk12student</t>
+  </si>
+  <si>
+    <t>fpadmin</t>
+  </si>
+  <si>
+    <t>qa</t>
+  </si>
+  <si>
+    <t>FPK12School6781</t>
+  </si>
+  <si>
+    <t>FPK12Classroom3937</t>
+  </si>
+  <si>
+    <t>FPK12Section144</t>
+  </si>
+  <si>
+    <t>5720</t>
+  </si>
+  <si>
+    <t>6428</t>
+  </si>
+  <si>
+    <t>2613</t>
+  </si>
+  <si>
+    <t>TestName</t>
+  </si>
+  <si>
+    <t>Automation Test</t>
+  </si>
+  <si>
+    <t>Grade</t>
+  </si>
+  <si>
+    <t>Subject</t>
+  </si>
+  <si>
+    <t>Grade 1</t>
+  </si>
+  <si>
+    <t>Assisted Reading</t>
+  </si>
+  <si>
+    <t>Grade 5</t>
+  </si>
+  <si>
+    <t>Calculus</t>
+  </si>
+  <si>
+    <t>Test For Automation</t>
+  </si>
+  <si>
     <t>automation</t>
   </si>
   <si>
     <t>ditrictadmin</t>
   </si>
   <si>
-    <t>@Abcd1234</t>
-  </si>
-  <si>
-    <t>password</t>
-  </si>
-  <si>
-    <t>fpk12admin</t>
-  </si>
-  <si>
-    <t>fpk12teacher</t>
-  </si>
-  <si>
-    <t>fpk12student</t>
-  </si>
-  <si>
-    <t>fpadmin</t>
-  </si>
-  <si>
-    <t>qa</t>
-  </si>
-  <si>
-    <t>FPK12School6781</t>
-  </si>
-  <si>
-    <t>FPK12Classroom3937</t>
-  </si>
-  <si>
-    <t>FPK12Section144</t>
-  </si>
-  <si>
-    <t>5720</t>
-  </si>
-  <si>
-    <t>6428</t>
-  </si>
-  <si>
-    <t>2613</t>
-  </si>
-  <si>
-    <t>TestName</t>
-  </si>
-  <si>
-    <t>Automation Test</t>
-  </si>
-  <si>
-    <t>Grade</t>
-  </si>
-  <si>
-    <t>Subject</t>
-  </si>
-  <si>
-    <t>Grade 1</t>
-  </si>
-  <si>
-    <t>Assisted Reading</t>
-  </si>
-  <si>
-    <t>Grade 5</t>
-  </si>
-  <si>
-    <t>Calculus</t>
-  </si>
-  <si>
-    <t>Test For Automation</t>
-  </si>
-  <si>
-    <t>FPK12Classroom41898</t>
-  </si>
-  <si>
-    <t>FPK12Section45697</t>
-  </si>
-  <si>
-    <t>FPK12School93938</t>
-  </si>
-  <si>
-    <t>66985</t>
-  </si>
-  <si>
-    <t>36009</t>
-  </si>
-  <si>
-    <t>46461</t>
-  </si>
-  <si>
-    <t>FPK12School24523</t>
-  </si>
-  <si>
-    <t>47523</t>
-  </si>
-  <si>
-    <t>0</t>
-  </si>
-  <si>
-    <t>95638</t>
-  </si>
-  <si>
-    <t>48045</t>
-  </si>
-  <si>
-    <t>FPK12School93651</t>
-  </si>
-  <si>
-    <t>FPK12Classroom85010</t>
-  </si>
-  <si>
-    <t>FPK12Section79808</t>
-  </si>
-  <si>
-    <t>40477</t>
-  </si>
-  <si>
-    <t>56244</t>
-  </si>
-  <si>
-    <t>53805</t>
-  </si>
-  <si>
-    <t>FPK12School56333</t>
-  </si>
-  <si>
-    <t>FPK12Classroom30485</t>
-  </si>
-  <si>
-    <t>FPK12Section88289</t>
+    <t>FPK12School65086</t>
+  </si>
+  <si>
+    <t>FPK12Classroom67383</t>
+  </si>
+  <si>
+    <t>FPK12Section65747</t>
+  </si>
+  <si>
+    <t>26235</t>
+  </si>
+  <si>
+    <t>58623</t>
+  </si>
+  <si>
+    <t>13127</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -255,7 +212,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -292,6 +249,19 @@
     <border>
       <left/>
       <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
         <color auto="1"/>
       </right>
       <top/>
@@ -300,19 +270,12 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <bottom style="thin"/>
-    </border>
-    <border>
-      <right style="thin"/>
-      <bottom style="thin"/>
-    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -370,32 +333,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyAlignment="true" applyBorder="true">
-      <alignment vertical="center" horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyAlignment="true" applyBorder="true">
-      <alignment vertical="center" horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyAlignment="true" applyBorder="true">
-      <alignment vertical="center" horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyAlignment="true" applyBorder="true">
-      <alignment vertical="center" horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyAlignment="true" applyBorder="true">
-      <alignment vertical="center" horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyAlignment="true" applyBorder="true">
-      <alignment vertical="center" horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyAlignment="true" applyBorder="true">
-      <alignment vertical="center" horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyAlignment="true" applyBorder="true">
-      <alignment vertical="center" horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyAlignment="true" applyBorder="true">
-      <alignment vertical="center" horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -413,6 +352,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -704,27 +647,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="30.0"/>
-    <col min="2" max="2" customWidth="true" width="23.5546875"/>
-    <col min="3" max="3" customWidth="true" width="24.77734375"/>
-    <col min="4" max="4" customWidth="true" style="1" width="19.88671875"/>
-    <col min="5" max="5" customWidth="true" style="1" width="23.77734375"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" style="1" width="20.5546875"/>
-    <col min="8" max="8" customWidth="true" width="31.5546875"/>
-    <col min="10" max="10" customWidth="true" width="19.77734375"/>
-    <col min="11" max="11" customWidth="true" width="15.0"/>
-    <col min="12" max="12" customWidth="true" width="18.33203125"/>
-    <col min="13" max="13" customWidth="true" width="19.33203125"/>
-    <col min="14" max="14" customWidth="true" width="23.6640625"/>
-    <col min="15" max="15" customWidth="true" width="20.109375"/>
-    <col min="16" max="16" customWidth="true" width="16.109375"/>
-    <col min="17" max="17" customWidth="true" width="15.0"/>
+    <col min="1" max="1" width="30" customWidth="1"/>
+    <col min="2" max="2" width="23.5546875" customWidth="1"/>
+    <col min="3" max="3" width="24.77734375" customWidth="1"/>
+    <col min="4" max="4" width="19.88671875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="23.77734375" style="1" customWidth="1"/>
+    <col min="7" max="7" width="20.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="31.5546875" customWidth="1"/>
+    <col min="10" max="10" width="19.77734375" customWidth="1"/>
+    <col min="11" max="11" width="15" customWidth="1"/>
+    <col min="12" max="12" width="18.33203125" customWidth="1"/>
+    <col min="13" max="13" width="19.33203125" customWidth="1"/>
+    <col min="14" max="14" width="23.6640625" customWidth="1"/>
+    <col min="15" max="15" width="20.109375" customWidth="1"/>
+    <col min="16" max="16" width="16.109375" customWidth="1"/>
+    <col min="17" max="17" width="15" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.3">
@@ -747,7 +690,7 @@
         <v>2</v>
       </c>
       <c r="G1" s="9" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="H1" s="11" t="s">
         <v>6</v>
@@ -756,39 +699,39 @@
         <v>8</v>
       </c>
       <c r="J1" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="K1" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="K1" s="19" t="s">
-        <v>26</v>
-      </c>
       <c r="L1" s="19" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="M1" s="10"/>
       <c r="N1" s="10"/>
       <c r="O1" s="10"/>
     </row>
     <row r="2" spans="1:18" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" t="s" s="27">
-        <v>50</v>
-      </c>
-      <c r="B2" t="s" s="28">
-        <v>51</v>
-      </c>
-      <c r="C2" t="s" s="29">
-        <v>52</v>
+      <c r="A2" s="21" t="s">
+        <v>33</v>
+      </c>
+      <c r="B2" s="21" t="s">
+        <v>34</v>
+      </c>
+      <c r="C2" s="21" t="s">
+        <v>35</v>
       </c>
       <c r="D2" s="13" t="s">
-        <v>9</v>
+        <v>31</v>
       </c>
       <c r="E2" s="13" t="s">
-        <v>10</v>
+        <v>32</v>
       </c>
       <c r="F2" s="13">
         <v>1323</v>
       </c>
       <c r="G2" s="13" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="H2" s="14" t="s">
         <v>7</v>
@@ -797,13 +740,13 @@
         <v>2024</v>
       </c>
       <c r="J2" s="13" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="K2" s="6" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="L2" s="6" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="M2" s="10"/>
       <c r="N2" s="10"/>
@@ -817,16 +760,16 @@
       <c r="B3" s="6"/>
       <c r="C3" s="6"/>
       <c r="D3" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="F3" s="13">
         <v>1323</v>
       </c>
       <c r="G3" s="13" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="H3" s="6"/>
       <c r="I3" s="6"/>
@@ -839,16 +782,16 @@
       <c r="B4" s="6"/>
       <c r="C4" s="6"/>
       <c r="D4" s="2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="F4" s="13">
+        <v>37</v>
+      </c>
+      <c r="F4" s="20">
         <v>1323</v>
       </c>
       <c r="G4" s="13" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="H4" s="6"/>
       <c r="I4" s="6"/>
@@ -861,16 +804,16 @@
       <c r="B5" s="13"/>
       <c r="C5" s="13"/>
       <c r="D5" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="F5" s="13">
+        <v>38</v>
+      </c>
+      <c r="F5" s="20">
         <v>1323</v>
       </c>
       <c r="G5" s="13" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="H5" s="6"/>
       <c r="I5" s="6"/>
@@ -908,16 +851,16 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="30.0"/>
-    <col min="2" max="2" customWidth="true" width="20.0"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="16.0"/>
-    <col min="4" max="4" customWidth="true" style="10" width="19.88671875"/>
-    <col min="5" max="5" customWidth="true" style="1" width="23.77734375"/>
-    <col min="7" max="7" customWidth="true" width="11.5546875"/>
-    <col min="8" max="8" customWidth="true" style="1" width="38.44140625"/>
-    <col min="11" max="11" customWidth="true" width="14.21875"/>
-    <col min="12" max="12" customWidth="true" width="15.0"/>
-    <col min="13" max="13" customWidth="true" width="18.33203125"/>
+    <col min="1" max="1" width="30" customWidth="1"/>
+    <col min="2" max="2" width="20" customWidth="1"/>
+    <col min="3" max="3" width="16" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.88671875" style="10" customWidth="1"/>
+    <col min="5" max="5" width="23.77734375" style="1" customWidth="1"/>
+    <col min="7" max="7" width="11.5546875" customWidth="1"/>
+    <col min="8" max="8" width="38.44140625" style="1" customWidth="1"/>
+    <col min="11" max="11" width="14.21875" customWidth="1"/>
+    <col min="12" max="12" width="15" customWidth="1"/>
+    <col min="13" max="13" width="18.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.3">
@@ -940,7 +883,7 @@
         <v>2</v>
       </c>
       <c r="G1" s="9" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="H1" s="11" t="s">
         <v>6</v>
@@ -949,37 +892,37 @@
         <v>8</v>
       </c>
       <c r="J1" s="19" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="K1" s="19" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="L1" s="18" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="M1" s="8"/>
     </row>
     <row r="2" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="B2" s="17" t="s">
-        <v>19</v>
-      </c>
-      <c r="C2" s="17" t="s">
-        <v>20</v>
-      </c>
       <c r="D2" s="10" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="F2" s="2">
         <v>242</v>
       </c>
       <c r="G2" s="13" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="H2" s="14" t="s">
         <v>7</v>
@@ -988,13 +931,13 @@
         <v>2024</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="L2" s="13" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="M2" s="3"/>
     </row>
@@ -1003,16 +946,16 @@
       <c r="B3" s="5"/>
       <c r="C3" s="5"/>
       <c r="D3" s="16" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="F3" s="2">
         <v>242</v>
       </c>
       <c r="G3" s="13" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="H3" s="6"/>
       <c r="I3" s="6"/>
@@ -1026,16 +969,16 @@
       <c r="B4" s="5"/>
       <c r="C4" s="5"/>
       <c r="D4" s="16" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="F4" s="2">
         <v>242</v>
       </c>
       <c r="G4" s="13" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="H4" s="6"/>
       <c r="I4" s="6"/>
@@ -1049,16 +992,16 @@
       <c r="B5" s="7"/>
       <c r="C5" s="7"/>
       <c r="D5" s="16" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="F5" s="2">
         <v>242</v>
       </c>
       <c r="G5" s="13" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="H5" s="6"/>
       <c r="I5" s="6"/>

</xml_diff>

<commit_message>
Parallel Execution Setup Configuratiopn code for Both modules
</commit_message>
<xml_diff>
--- a/src/test/resources/ExcelFiles/AssessmentCenterDetails.xlsx
+++ b/src/test/resources/ExcelFiles/AssessmentCenterDetails.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="146">
   <si>
     <t>FirstName</t>
   </si>
@@ -174,6 +174,291 @@
   </si>
   <si>
     <t>707906</t>
+  </si>
+  <si>
+    <t>FPK12School834302</t>
+  </si>
+  <si>
+    <t>FPK12Classroom899844</t>
+  </si>
+  <si>
+    <t>FPK12Section655097</t>
+  </si>
+  <si>
+    <t>FPK12School874444</t>
+  </si>
+  <si>
+    <t>FPK12Classroom817792</t>
+  </si>
+  <si>
+    <t>FPK12Section662097</t>
+  </si>
+  <si>
+    <t>FPK12School472470</t>
+  </si>
+  <si>
+    <t>FPK12Classroom185526</t>
+  </si>
+  <si>
+    <t>FPK12Section28367</t>
+  </si>
+  <si>
+    <t>138299</t>
+  </si>
+  <si>
+    <t>668571</t>
+  </si>
+  <si>
+    <t>FPK12School570277</t>
+  </si>
+  <si>
+    <t>FPK12Classroom971132</t>
+  </si>
+  <si>
+    <t>FPK12Section740945</t>
+  </si>
+  <si>
+    <t>815337</t>
+  </si>
+  <si>
+    <t>FPK12School414238</t>
+  </si>
+  <si>
+    <t>FPK12Classroom197410</t>
+  </si>
+  <si>
+    <t>FPK12Section911582</t>
+  </si>
+  <si>
+    <t>210904</t>
+  </si>
+  <si>
+    <t>475463</t>
+  </si>
+  <si>
+    <t>91303</t>
+  </si>
+  <si>
+    <t>FPK12School244016</t>
+  </si>
+  <si>
+    <t>FPK12Classroom526964</t>
+  </si>
+  <si>
+    <t>FPK12Section966301</t>
+  </si>
+  <si>
+    <t>316790</t>
+  </si>
+  <si>
+    <t>FPK12School632679</t>
+  </si>
+  <si>
+    <t>FPK12Classroom475626</t>
+  </si>
+  <si>
+    <t>FPK12Section712338</t>
+  </si>
+  <si>
+    <t>56766</t>
+  </si>
+  <si>
+    <t>FPK12School821642</t>
+  </si>
+  <si>
+    <t>FPK12Classroom566948</t>
+  </si>
+  <si>
+    <t>FPK12Section493845</t>
+  </si>
+  <si>
+    <t>FPK12School159261</t>
+  </si>
+  <si>
+    <t>FPK12Classroom30584</t>
+  </si>
+  <si>
+    <t>FPK12Section606442</t>
+  </si>
+  <si>
+    <t>305970</t>
+  </si>
+  <si>
+    <t>FPK12School678415</t>
+  </si>
+  <si>
+    <t>FPK12Classroom891335</t>
+  </si>
+  <si>
+    <t>FPK12Section153893</t>
+  </si>
+  <si>
+    <t>867475</t>
+  </si>
+  <si>
+    <t>FPK12School799268</t>
+  </si>
+  <si>
+    <t>FPK12Classroom627904</t>
+  </si>
+  <si>
+    <t>FPK12Section890745</t>
+  </si>
+  <si>
+    <t>FPK12School709263</t>
+  </si>
+  <si>
+    <t>FPK12Classroom514145</t>
+  </si>
+  <si>
+    <t>FPK12Section69949</t>
+  </si>
+  <si>
+    <t>FPK12School890941</t>
+  </si>
+  <si>
+    <t>FPK12Classroom209284</t>
+  </si>
+  <si>
+    <t>FPK12Section932503</t>
+  </si>
+  <si>
+    <t>FPK12School571406</t>
+  </si>
+  <si>
+    <t>FPK12Classroom185032</t>
+  </si>
+  <si>
+    <t>FPK12Section329845</t>
+  </si>
+  <si>
+    <t>FPK12School611483</t>
+  </si>
+  <si>
+    <t>FPK12Classroom570221</t>
+  </si>
+  <si>
+    <t>FPK12Section52194</t>
+  </si>
+  <si>
+    <t>FPK12School574299</t>
+  </si>
+  <si>
+    <t>FPK12Classroom857788</t>
+  </si>
+  <si>
+    <t>FPK12Section616591</t>
+  </si>
+  <si>
+    <t>FPK12School67179</t>
+  </si>
+  <si>
+    <t>FPK12Classroom209731</t>
+  </si>
+  <si>
+    <t>FPK12Section628126</t>
+  </si>
+  <si>
+    <t>FPK12School277228</t>
+  </si>
+  <si>
+    <t>FPK12Classroom6375</t>
+  </si>
+  <si>
+    <t>FPK12Section58795</t>
+  </si>
+  <si>
+    <t>61388</t>
+  </si>
+  <si>
+    <t>FPK12School159566</t>
+  </si>
+  <si>
+    <t>FPK12Classroom328856</t>
+  </si>
+  <si>
+    <t>FPK12Section496227</t>
+  </si>
+  <si>
+    <t>216356</t>
+  </si>
+  <si>
+    <t>446216</t>
+  </si>
+  <si>
+    <t>931198</t>
+  </si>
+  <si>
+    <t>FPK12School681521</t>
+  </si>
+  <si>
+    <t>FPK12Classroom914925</t>
+  </si>
+  <si>
+    <t>FPK12Section619913</t>
+  </si>
+  <si>
+    <t>348588</t>
+  </si>
+  <si>
+    <t>192928</t>
+  </si>
+  <si>
+    <t>61758</t>
+  </si>
+  <si>
+    <t>FPK12School164532</t>
+  </si>
+  <si>
+    <t>FPK12Classroom689022</t>
+  </si>
+  <si>
+    <t>FPK12Section602519</t>
+  </si>
+  <si>
+    <t>561005</t>
+  </si>
+  <si>
+    <t>274631</t>
+  </si>
+  <si>
+    <t>882491</t>
+  </si>
+  <si>
+    <t>FPK12School153995</t>
+  </si>
+  <si>
+    <t>FPK12Classroom357376</t>
+  </si>
+  <si>
+    <t>FPK12Section608390</t>
+  </si>
+  <si>
+    <t>803723</t>
+  </si>
+  <si>
+    <t>339821</t>
+  </si>
+  <si>
+    <t>926187</t>
+  </si>
+  <si>
+    <t>FPK12School645306</t>
+  </si>
+  <si>
+    <t>FPK12Classroom303103</t>
+  </si>
+  <si>
+    <t>FPK12Section768697</t>
+  </si>
+  <si>
+    <t>324719</t>
+  </si>
+  <si>
+    <t>640224</t>
+  </si>
+  <si>
+    <t>197715</t>
   </si>
 </sst>
 </file>
@@ -319,7 +604,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="97">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -379,6 +664,213 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyAlignment="true" applyBorder="true">
       <alignment vertical="center" horizontal="center"/>
@@ -770,14 +1262,14 @@
       <c r="O1" s="10"/>
     </row>
     <row r="2" spans="1:18" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" t="s" s="25">
-        <v>45</v>
-      </c>
-      <c r="B2" t="s" s="26">
-        <v>46</v>
-      </c>
-      <c r="C2" t="s" s="27">
-        <v>47</v>
+      <c r="A2" t="s" s="94">
+        <v>140</v>
+      </c>
+      <c r="B2" t="s" s="95">
+        <v>141</v>
+      </c>
+      <c r="C2" t="s" s="96">
+        <v>142</v>
       </c>
       <c r="D2" s="13" t="s">
         <v>30</v>
@@ -821,7 +1313,7 @@
         <v>11</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>48</v>
+        <v>143</v>
       </c>
       <c r="F3" s="13">
         <v>1323</v>
@@ -843,7 +1335,7 @@
         <v>12</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>49</v>
+        <v>144</v>
       </c>
       <c r="F4" s="20">
         <v>1323</v>
@@ -865,7 +1357,7 @@
         <v>13</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>50</v>
+        <v>145</v>
       </c>
       <c r="F5" s="20">
         <v>1323</v>

</xml_diff>

<commit_message>
Timeout Exception Handling Code
</commit_message>
<xml_diff>
--- a/src/test/resources/ExcelFiles/AssessmentCenterDetails.xlsx
+++ b/src/test/resources/ExcelFiles/AssessmentCenterDetails.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="344" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="362" uniqueCount="170">
   <si>
     <t>FirstName</t>
   </si>
@@ -513,6 +513,24 @@
   </si>
   <si>
     <t>619371</t>
+  </si>
+  <si>
+    <t>FPK12School304</t>
+  </si>
+  <si>
+    <t>FPK12Classroom829407</t>
+  </si>
+  <si>
+    <t>FPK12Section211134</t>
+  </si>
+  <si>
+    <t>643169</t>
+  </si>
+  <si>
+    <t>634111</t>
+  </si>
+  <si>
+    <t>477830</t>
   </si>
 </sst>
 </file>
@@ -658,7 +676,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="106">
+  <cellXfs count="109">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -718,6 +736,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyAlignment="true" applyBorder="true">
       <alignment vertical="center" horizontal="center"/>
@@ -1343,14 +1370,14 @@
       <c r="O1" s="10"/>
     </row>
     <row r="2" spans="1:18" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" t="s" s="103">
-        <v>158</v>
-      </c>
-      <c r="B2" t="s" s="104">
-        <v>159</v>
-      </c>
-      <c r="C2" t="s" s="105">
-        <v>160</v>
+      <c r="A2" t="s" s="106">
+        <v>164</v>
+      </c>
+      <c r="B2" t="s" s="107">
+        <v>165</v>
+      </c>
+      <c r="C2" t="s" s="108">
+        <v>166</v>
       </c>
       <c r="D2" s="13" t="s">
         <v>30</v>
@@ -1394,7 +1421,7 @@
         <v>11</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>161</v>
+        <v>167</v>
       </c>
       <c r="F3" s="13">
         <v>1323</v>
@@ -1416,7 +1443,7 @@
         <v>12</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>162</v>
+        <v>168</v>
       </c>
       <c r="F4" s="20">
         <v>1323</v>
@@ -1438,7 +1465,7 @@
         <v>13</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>163</v>
+        <v>169</v>
       </c>
       <c r="F5" s="20">
         <v>1323</v>

</xml_diff>

<commit_message>
Updated Sections creation Code
</commit_message>
<xml_diff>
--- a/src/test/resources/ExcelFiles/AssessmentCenterDetails.xlsx
+++ b/src/test/resources/ExcelFiles/AssessmentCenterDetails.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="398" uniqueCount="182">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="411" uniqueCount="192">
   <si>
     <t>FirstName</t>
   </si>
@@ -567,6 +567,36 @@
   </si>
   <si>
     <t>115511</t>
+  </si>
+  <si>
+    <t>FPK12School675931</t>
+  </si>
+  <si>
+    <t>FPK12Classroom502606</t>
+  </si>
+  <si>
+    <t>FPK12Section57566</t>
+  </si>
+  <si>
+    <t>194088</t>
+  </si>
+  <si>
+    <t>FPK12School876300</t>
+  </si>
+  <si>
+    <t>FPK12Classroom99623</t>
+  </si>
+  <si>
+    <t>FPK12Section82432</t>
+  </si>
+  <si>
+    <t>FPK12School37228</t>
+  </si>
+  <si>
+    <t>FPK12Classroom612221</t>
+  </si>
+  <si>
+    <t>FPK12Section719288</t>
   </si>
 </sst>
 </file>
@@ -712,7 +742,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="115">
+  <cellXfs count="124">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -772,6 +802,33 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyAlignment="true" applyBorder="true">
       <alignment vertical="center" horizontal="center"/>
@@ -1424,14 +1481,14 @@
       <c r="O1" s="10"/>
     </row>
     <row r="2" spans="1:18" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" t="s" s="112">
-        <v>176</v>
-      </c>
-      <c r="B2" t="s" s="113">
-        <v>177</v>
-      </c>
-      <c r="C2" t="s" s="114">
-        <v>178</v>
+      <c r="A2" t="s" s="121">
+        <v>189</v>
+      </c>
+      <c r="B2" t="s" s="122">
+        <v>190</v>
+      </c>
+      <c r="C2" t="s" s="123">
+        <v>191</v>
       </c>
       <c r="D2" s="13" t="s">
         <v>30</v>
@@ -1475,7 +1532,7 @@
         <v>11</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>179</v>
+        <v>185</v>
       </c>
       <c r="F3" s="13">
         <v>1323</v>
@@ -1493,11 +1550,9 @@
       <c r="A4" s="6"/>
       <c r="B4" s="6"/>
       <c r="C4" s="6"/>
-      <c r="D4" s="2" t="s">
-        <v>12</v>
-      </c>
+      <c r="D4" s="2"/>
       <c r="E4" s="2" t="s">
-        <v>180</v>
+        <v>42</v>
       </c>
       <c r="F4" s="20">
         <v>1323</v>
@@ -1515,11 +1570,9 @@
       <c r="A5" s="13"/>
       <c r="B5" s="13"/>
       <c r="C5" s="13"/>
-      <c r="D5" s="2" t="s">
-        <v>13</v>
-      </c>
+      <c r="D5" s="2"/>
       <c r="E5" s="2" t="s">
-        <v>181</v>
+        <v>42</v>
       </c>
       <c r="F5" s="20">
         <v>1323</v>

</xml_diff>

<commit_message>
Common pages making Global class
</commit_message>
<xml_diff>
--- a/src/test/resources/ExcelFiles/AssessmentCenterDetails.xlsx
+++ b/src/test/resources/ExcelFiles/AssessmentCenterDetails.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="411" uniqueCount="192">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="519" uniqueCount="240">
   <si>
     <t>FirstName</t>
   </si>
@@ -597,6 +597,150 @@
   </si>
   <si>
     <t>FPK12Section719288</t>
+  </si>
+  <si>
+    <t>FPK12School785589</t>
+  </si>
+  <si>
+    <t>FPK12Classroom965019</t>
+  </si>
+  <si>
+    <t>FPK12Section110326</t>
+  </si>
+  <si>
+    <t>FPK12School242544</t>
+  </si>
+  <si>
+    <t>FPK12Classroom318749</t>
+  </si>
+  <si>
+    <t>FPK12Section976263</t>
+  </si>
+  <si>
+    <t>FPK12School549941</t>
+  </si>
+  <si>
+    <t>FPK12Classroom96157</t>
+  </si>
+  <si>
+    <t>FPK12Section792294</t>
+  </si>
+  <si>
+    <t>FPK12School485756</t>
+  </si>
+  <si>
+    <t>FPK12Classroom265171</t>
+  </si>
+  <si>
+    <t>FPK12Section956595</t>
+  </si>
+  <si>
+    <t>FPK12School405575</t>
+  </si>
+  <si>
+    <t>FPK12Classroom808049</t>
+  </si>
+  <si>
+    <t>FPK12Section893145</t>
+  </si>
+  <si>
+    <t>FPK12School141838</t>
+  </si>
+  <si>
+    <t>FPK12Classroom140958</t>
+  </si>
+  <si>
+    <t>FPK12Section738767</t>
+  </si>
+  <si>
+    <t>637109</t>
+  </si>
+  <si>
+    <t>124719</t>
+  </si>
+  <si>
+    <t>959574</t>
+  </si>
+  <si>
+    <t>FPK12School139160</t>
+  </si>
+  <si>
+    <t>FPK12Classroom727679</t>
+  </si>
+  <si>
+    <t>FPK12Section821928</t>
+  </si>
+  <si>
+    <t>700979</t>
+  </si>
+  <si>
+    <t>158683</t>
+  </si>
+  <si>
+    <t>739998</t>
+  </si>
+  <si>
+    <t>FPK12School704362</t>
+  </si>
+  <si>
+    <t>FPK12Classroom421451</t>
+  </si>
+  <si>
+    <t>FPK12Section39302</t>
+  </si>
+  <si>
+    <t>155379</t>
+  </si>
+  <si>
+    <t>236053</t>
+  </si>
+  <si>
+    <t>773925</t>
+  </si>
+  <si>
+    <t>FPK12School602302</t>
+  </si>
+  <si>
+    <t>FPK12Classroom732590</t>
+  </si>
+  <si>
+    <t>FPK12Section408551</t>
+  </si>
+  <si>
+    <t>FPK12School296618</t>
+  </si>
+  <si>
+    <t>FPK12Classroom322583</t>
+  </si>
+  <si>
+    <t>FPK12Section530882</t>
+  </si>
+  <si>
+    <t>958460</t>
+  </si>
+  <si>
+    <t>591823</t>
+  </si>
+  <si>
+    <t>578312</t>
+  </si>
+  <si>
+    <t>FPK12School997175</t>
+  </si>
+  <si>
+    <t>FPK12Classroom620922</t>
+  </si>
+  <si>
+    <t>FPK12Section947416</t>
+  </si>
+  <si>
+    <t>119789</t>
+  </si>
+  <si>
+    <t>300105</t>
+  </si>
+  <si>
+    <t>79112</t>
   </si>
 </sst>
 </file>
@@ -742,7 +886,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="124">
+  <cellXfs count="157">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -802,6 +946,105 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyAlignment="true" applyBorder="true">
       <alignment vertical="center" horizontal="center"/>
@@ -1481,14 +1724,14 @@
       <c r="O1" s="10"/>
     </row>
     <row r="2" spans="1:18" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" t="s" s="121">
-        <v>189</v>
-      </c>
-      <c r="B2" t="s" s="122">
-        <v>190</v>
-      </c>
-      <c r="C2" t="s" s="123">
-        <v>191</v>
+      <c r="A2" t="s" s="154">
+        <v>234</v>
+      </c>
+      <c r="B2" t="s" s="155">
+        <v>235</v>
+      </c>
+      <c r="C2" t="s" s="156">
+        <v>236</v>
       </c>
       <c r="D2" s="13" t="s">
         <v>30</v>
@@ -1532,7 +1775,7 @@
         <v>11</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>185</v>
+        <v>237</v>
       </c>
       <c r="F3" s="13">
         <v>1323</v>
@@ -1550,9 +1793,11 @@
       <c r="A4" s="6"/>
       <c r="B4" s="6"/>
       <c r="C4" s="6"/>
-      <c r="D4" s="2"/>
+      <c r="D4" s="2" t="s">
+        <v>12</v>
+      </c>
       <c r="E4" s="2" t="s">
-        <v>42</v>
+        <v>238</v>
       </c>
       <c r="F4" s="20">
         <v>1323</v>
@@ -1570,9 +1815,11 @@
       <c r="A5" s="13"/>
       <c r="B5" s="13"/>
       <c r="C5" s="13"/>
-      <c r="D5" s="2"/>
+      <c r="D5" s="2" t="s">
+        <v>13</v>
+      </c>
       <c r="E5" s="2" t="s">
-        <v>42</v>
+        <v>239</v>
       </c>
       <c r="F5" s="20">
         <v>1323</v>

</xml_diff>

<commit_message>
Retry Mechanism added for Section Saving
</commit_message>
<xml_diff>
--- a/src/test/resources/ExcelFiles/AssessmentCenterDetails.xlsx
+++ b/src/test/resources/ExcelFiles/AssessmentCenterDetails.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="831" uniqueCount="374">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="861" uniqueCount="392">
   <si>
     <t>FirstName</t>
   </si>
@@ -1143,6 +1143,60 @@
   </si>
   <si>
     <t>676095</t>
+  </si>
+  <si>
+    <t>FPK12School51997</t>
+  </si>
+  <si>
+    <t>FPK12Classroom9537</t>
+  </si>
+  <si>
+    <t>FPK12Section931393</t>
+  </si>
+  <si>
+    <t>FPK12Section826703</t>
+  </si>
+  <si>
+    <t>631473</t>
+  </si>
+  <si>
+    <t>926821</t>
+  </si>
+  <si>
+    <t>975854</t>
+  </si>
+  <si>
+    <t>FPK12School508757</t>
+  </si>
+  <si>
+    <t>FPK12Classroom148497</t>
+  </si>
+  <si>
+    <t>FPK12Section874489</t>
+  </si>
+  <si>
+    <t>FPK12School307650</t>
+  </si>
+  <si>
+    <t>FPK12Classroom569237</t>
+  </si>
+  <si>
+    <t>FPK12Section399549</t>
+  </si>
+  <si>
+    <t>FPK12School819492</t>
+  </si>
+  <si>
+    <t>FPK12Classroom284587</t>
+  </si>
+  <si>
+    <t>FPK12Section593997</t>
+  </si>
+  <si>
+    <t>FPK12Section187298</t>
+  </si>
+  <si>
+    <t>FPK12Section290547</t>
   </si>
 </sst>
 </file>
@@ -1288,7 +1342,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="245">
+  <cellXfs count="260">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1348,6 +1402,51 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyAlignment="true" applyBorder="true">
       <alignment vertical="center" horizontal="center"/>
@@ -2390,14 +2489,14 @@
       <c r="O1" s="10"/>
     </row>
     <row r="2" spans="1:18" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" t="s" s="241">
-        <v>367</v>
-      </c>
-      <c r="B2" t="s" s="242">
-        <v>368</v>
-      </c>
-      <c r="C2" t="s" s="244">
-        <v>370</v>
+      <c r="A2" t="s" s="255">
+        <v>387</v>
+      </c>
+      <c r="B2" t="s" s="256">
+        <v>388</v>
+      </c>
+      <c r="C2" t="s" s="259">
+        <v>391</v>
       </c>
       <c r="D2" s="13" t="s">
         <v>30</v>
@@ -2441,7 +2540,7 @@
         <v>11</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>371</v>
+        <v>378</v>
       </c>
       <c r="F3" s="13">
         <v>1323</v>
@@ -2463,7 +2562,7 @@
         <v>12</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>372</v>
+        <v>379</v>
       </c>
       <c r="F4" s="20">
         <v>1323</v>
@@ -2485,7 +2584,7 @@
         <v>13</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>373</v>
+        <v>380</v>
       </c>
       <c r="F5" s="20">
         <v>1323</v>

</xml_diff>

<commit_message>
Location Creation Script changes
</commit_message>
<xml_diff>
--- a/src/test/resources/ExcelFiles/AssessmentCenterDetails.xlsx
+++ b/src/test/resources/ExcelFiles/AssessmentCenterDetails.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="861" uniqueCount="392">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="879" uniqueCount="398">
   <si>
     <t>FirstName</t>
   </si>
@@ -1197,6 +1197,24 @@
   </si>
   <si>
     <t>FPK12Section290547</t>
+  </si>
+  <si>
+    <t>FPK12School324596</t>
+  </si>
+  <si>
+    <t>FPK12Classroom23919</t>
+  </si>
+  <si>
+    <t>FPK12Section854087</t>
+  </si>
+  <si>
+    <t>467085</t>
+  </si>
+  <si>
+    <t>599077</t>
+  </si>
+  <si>
+    <t>998932</t>
   </si>
 </sst>
 </file>
@@ -1342,7 +1360,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="260">
+  <cellXfs count="263">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1402,6 +1420,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyAlignment="true" applyBorder="true">
       <alignment vertical="center" horizontal="center"/>
@@ -2489,14 +2516,14 @@
       <c r="O1" s="10"/>
     </row>
     <row r="2" spans="1:18" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" t="s" s="255">
-        <v>387</v>
-      </c>
-      <c r="B2" t="s" s="256">
-        <v>388</v>
-      </c>
-      <c r="C2" t="s" s="259">
-        <v>391</v>
+      <c r="A2" t="s" s="260">
+        <v>392</v>
+      </c>
+      <c r="B2" t="s" s="261">
+        <v>393</v>
+      </c>
+      <c r="C2" t="s" s="262">
+        <v>394</v>
       </c>
       <c r="D2" s="13" t="s">
         <v>30</v>
@@ -2540,7 +2567,7 @@
         <v>11</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>378</v>
+        <v>395</v>
       </c>
       <c r="F3" s="13">
         <v>1323</v>
@@ -2562,7 +2589,7 @@
         <v>12</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>379</v>
+        <v>396</v>
       </c>
       <c r="F4" s="20">
         <v>1323</v>
@@ -2584,7 +2611,7 @@
         <v>13</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>380</v>
+        <v>397</v>
       </c>
       <c r="F5" s="20">
         <v>1323</v>

</xml_diff>

<commit_message>
Award badge Code & Announcements Scripts Enhancements
</commit_message>
<xml_diff>
--- a/src/test/resources/ExcelFiles/AssessmentCenterDetails.xlsx
+++ b/src/test/resources/ExcelFiles/AssessmentCenterDetails.xlsx
@@ -1,27 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28429"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Focalpoint Automation\FPK12AutomationProject\src\test\resources\ExcelFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D2ACDDE-55D9-40BB-B114-C26B18E6F2EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11588D5E-DDBF-4F6A-B3DD-5F898FA07FAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1848" yWindow="1848" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="STAGE" sheetId="1" r:id="rId1"/>
-    <sheet name="LMSProd" sheetId="3" r:id="rId2"/>
+    <sheet name="DEMO" sheetId="4" r:id="rId2"/>
+    <sheet name="LMSProd" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="43">
   <si>
     <t>FirstName</t>
   </si>
@@ -119,72 +120,44 @@
     <t>ditrictadmin</t>
   </si>
   <si>
-    <t>27065</t>
-  </si>
-  <si>
-    <t>1817</t>
-  </si>
-  <si>
-    <t>FPK12Classroom2428</t>
-  </si>
-  <si>
-    <t>FPK12Section315</t>
-  </si>
-  <si>
-    <t>FPK12School8204</t>
-  </si>
-  <si>
-    <t>FPK12School63240</t>
-  </si>
-  <si>
-    <t>FPK12Classroom18566</t>
-  </si>
-  <si>
-    <t>FPK12Section99767</t>
-  </si>
-  <si>
-    <t>30885</t>
+    <t>testdemo</t>
+  </si>
+  <si>
+    <t>test1</t>
   </si>
   <si>
     <t>0</t>
   </si>
   <si>
-    <t>81114</t>
-  </si>
-  <si>
-    <t>FPK12School53823</t>
-  </si>
-  <si>
-    <t>FPK12Classroom18487</t>
-  </si>
-  <si>
-    <t>FPK12Section5668</t>
-  </si>
-  <si>
-    <t>FPK12School37329</t>
-  </si>
-  <si>
-    <t>FPK12Classroom73671</t>
-  </si>
-  <si>
-    <t>FPK12Section31330</t>
-  </si>
-  <si>
-    <t>76366</t>
-  </si>
-  <si>
-    <t>18970</t>
-  </si>
-  <si>
-    <t>10486</t>
+    <t>FPK12School86218</t>
+  </si>
+  <si>
+    <t>FPK12Classroom75168</t>
+  </si>
+  <si>
+    <t>FPK12Section74975</t>
+  </si>
+  <si>
+    <t>77893</t>
+  </si>
+  <si>
+    <t>FPK12Classroom91971</t>
+  </si>
+  <si>
+    <t>FPK12Section22464</t>
+  </si>
+  <si>
+    <t>FPK12School34583</t>
+  </si>
+  <si>
+    <t>9643</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -225,6 +198,18 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF009688"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF333335"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -252,7 +237,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -310,19 +295,12 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <bottom style="thin"/>
-    </border>
-    <border>
-      <right style="thin"/>
-      <bottom style="thin"/>
-    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -383,33 +361,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyAlignment="true" applyBorder="true">
-      <alignment vertical="center" horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyAlignment="true" applyBorder="true">
-      <alignment vertical="center" horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyAlignment="true" applyBorder="true">
-      <alignment vertical="center" horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyAlignment="true" applyBorder="true">
-      <alignment vertical="center" horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyAlignment="true" applyBorder="true">
-      <alignment vertical="center" horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyAlignment="true" applyBorder="true">
-      <alignment vertical="center" horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyAlignment="true" applyBorder="true">
-      <alignment vertical="center" horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyAlignment="true" applyBorder="true">
-      <alignment vertical="center" horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyAlignment="true" applyBorder="true">
-      <alignment vertical="center" horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -718,26 +671,26 @@
   <dimension ref="A1:R6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="30.0"/>
-    <col min="2" max="2" customWidth="true" width="23.5546875"/>
-    <col min="3" max="3" customWidth="true" width="24.77734375"/>
-    <col min="4" max="4" customWidth="true" style="1" width="19.88671875"/>
-    <col min="5" max="5" customWidth="true" style="1" width="23.77734375"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" style="1" width="20.5546875"/>
-    <col min="8" max="8" customWidth="true" width="31.5546875"/>
-    <col min="10" max="10" customWidth="true" width="19.77734375"/>
-    <col min="11" max="11" customWidth="true" width="15.0"/>
-    <col min="12" max="12" customWidth="true" width="18.33203125"/>
-    <col min="13" max="13" customWidth="true" width="19.33203125"/>
-    <col min="14" max="14" customWidth="true" width="23.6640625"/>
-    <col min="15" max="15" customWidth="true" width="20.109375"/>
-    <col min="16" max="16" customWidth="true" width="16.109375"/>
-    <col min="17" max="17" customWidth="true" width="15.0"/>
+    <col min="1" max="1" width="30" customWidth="1"/>
+    <col min="2" max="2" width="23.5546875" customWidth="1"/>
+    <col min="3" max="3" width="24.77734375" customWidth="1"/>
+    <col min="4" max="4" width="19.88671875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="23.77734375" style="1" customWidth="1"/>
+    <col min="7" max="7" width="20.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="31.5546875" customWidth="1"/>
+    <col min="10" max="10" width="19.77734375" customWidth="1"/>
+    <col min="11" max="11" width="15" customWidth="1"/>
+    <col min="12" max="12" width="18.33203125" customWidth="1"/>
+    <col min="13" max="13" width="19.33203125" customWidth="1"/>
+    <col min="14" max="14" width="23.6640625" customWidth="1"/>
+    <col min="15" max="15" width="20.109375" customWidth="1"/>
+    <col min="16" max="16" width="16.109375" customWidth="1"/>
+    <col min="17" max="17" width="15" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.3">
@@ -782,14 +735,14 @@
       <c r="O1" s="10"/>
     </row>
     <row r="2" spans="1:18" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" t="s" s="28">
-        <v>46</v>
-      </c>
-      <c r="B2" t="s" s="29">
-        <v>47</v>
-      </c>
-      <c r="C2" t="s" s="30">
-        <v>48</v>
+      <c r="A2" s="21" t="s">
+        <v>41</v>
+      </c>
+      <c r="B2" s="23" t="s">
+        <v>39</v>
+      </c>
+      <c r="C2" s="23" t="s">
+        <v>40</v>
       </c>
       <c r="D2" s="13" t="s">
         <v>30</v>
@@ -833,7 +786,7 @@
         <v>11</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="F3" s="13">
         <v>1323</v>
@@ -854,8 +807,8 @@
       <c r="D4" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="E4" s="2" t="s">
-        <v>50</v>
+      <c r="E4" s="22">
+        <v>5403</v>
       </c>
       <c r="F4" s="20">
         <v>1323</v>
@@ -876,8 +829,8 @@
       <c r="D5" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="E5" s="2" t="s">
-        <v>51</v>
+      <c r="E5" s="2">
+        <v>65936</v>
       </c>
       <c r="F5" s="20">
         <v>1323</v>
@@ -912,6 +865,194 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{083A40E5-8962-4454-A5E1-8BADF1ED1E37}">
+  <dimension ref="A1:R6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H10" sqref="H10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="16.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.77734375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.77734375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.77734375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="27.5546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7.33203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="8" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="K1" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="L1" s="19" t="s">
+        <v>25</v>
+      </c>
+      <c r="M1" s="10"/>
+      <c r="N1" s="10"/>
+      <c r="O1" s="10"/>
+    </row>
+    <row r="2" spans="1:18" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="21" t="s">
+        <v>35</v>
+      </c>
+      <c r="B2" s="21" t="s">
+        <v>36</v>
+      </c>
+      <c r="C2" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="D2" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="E2" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="F2" s="13">
+        <v>2</v>
+      </c>
+      <c r="G2" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="H2" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="I2" s="13">
+        <v>2024</v>
+      </c>
+      <c r="J2" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="K2" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="L2" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="M2" s="10"/>
+      <c r="N2" s="10"/>
+      <c r="O2" s="10"/>
+      <c r="P2" s="10"/>
+      <c r="Q2" s="10"/>
+      <c r="R2" s="10"/>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A3" s="6"/>
+      <c r="B3" s="6"/>
+      <c r="C3" s="6"/>
+      <c r="D3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="F3" s="13">
+        <v>2</v>
+      </c>
+      <c r="G3" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="H3" s="6"/>
+      <c r="I3" s="6"/>
+      <c r="J3" s="6"/>
+      <c r="K3" s="6"/>
+      <c r="L3" s="6"/>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A4" s="6"/>
+      <c r="B4" s="6"/>
+      <c r="C4" s="6"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="F4" s="13">
+        <v>2</v>
+      </c>
+      <c r="G4" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="H4" s="6"/>
+      <c r="I4" s="6"/>
+      <c r="J4" s="6"/>
+      <c r="K4" s="6"/>
+      <c r="L4" s="6"/>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A5" s="13"/>
+      <c r="B5" s="13"/>
+      <c r="C5" s="13"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="F5" s="13">
+        <v>2</v>
+      </c>
+      <c r="G5" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="H5" s="6"/>
+      <c r="I5" s="6"/>
+      <c r="J5" s="6"/>
+      <c r="K5" s="6"/>
+      <c r="L5" s="6"/>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A6" s="13"/>
+      <c r="B6" s="13"/>
+      <c r="C6" s="13"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="6"/>
+      <c r="G6" s="2"/>
+      <c r="H6" s="6"/>
+      <c r="I6" s="6"/>
+      <c r="J6" s="6"/>
+      <c r="K6" s="6"/>
+      <c r="L6" s="6"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:M6"/>
   <sheetViews>
@@ -921,16 +1062,16 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="30.0"/>
-    <col min="2" max="2" customWidth="true" width="20.0"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="16.0"/>
-    <col min="4" max="4" customWidth="true" style="10" width="19.88671875"/>
-    <col min="5" max="5" customWidth="true" style="1" width="23.77734375"/>
-    <col min="7" max="7" customWidth="true" width="11.5546875"/>
-    <col min="8" max="8" customWidth="true" style="1" width="38.44140625"/>
-    <col min="11" max="11" customWidth="true" width="14.21875"/>
-    <col min="12" max="12" customWidth="true" width="15.0"/>
-    <col min="13" max="13" customWidth="true" width="18.33203125"/>
+    <col min="1" max="1" width="30" customWidth="1"/>
+    <col min="2" max="2" width="20" customWidth="1"/>
+    <col min="3" max="3" width="16" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.88671875" style="10" customWidth="1"/>
+    <col min="5" max="5" width="23.77734375" style="1" customWidth="1"/>
+    <col min="7" max="7" width="11.5546875" customWidth="1"/>
+    <col min="8" max="8" width="38.44140625" style="1" customWidth="1"/>
+    <col min="11" max="11" width="14.21875" customWidth="1"/>
+    <col min="12" max="12" width="15" customWidth="1"/>
+    <col min="13" max="13" width="18.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Logics added for Searching the Community in Portfolio
</commit_message>
<xml_diff>
--- a/src/test/resources/ExcelFiles/AssessmentCenterDetails.xlsx
+++ b/src/test/resources/ExcelFiles/AssessmentCenterDetails.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="57">
   <si>
     <t>FirstName</t>
   </si>
@@ -169,6 +169,30 @@
   </si>
   <si>
     <t>83442</t>
+  </si>
+  <si>
+    <t>FPK12School82076</t>
+  </si>
+  <si>
+    <t>FPK12Classroom82865</t>
+  </si>
+  <si>
+    <t>FPK12Section14416</t>
+  </si>
+  <si>
+    <t>FPK12Section75560</t>
+  </si>
+  <si>
+    <t>FPK12Section39584</t>
+  </si>
+  <si>
+    <t>67807</t>
+  </si>
+  <si>
+    <t>21227</t>
+  </si>
+  <si>
+    <t>34255</t>
   </si>
 </sst>
 </file>
@@ -326,7 +350,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -389,6 +413,21 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyAlignment="true" applyBorder="true">
       <alignment vertical="center" horizontal="center"/>
     </xf>
@@ -770,14 +809,14 @@
       <c r="O1" s="10"/>
     </row>
     <row r="2" spans="1:18" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" t="s" s="24">
-        <v>43</v>
-      </c>
-      <c r="B2" t="s" s="25">
-        <v>44</v>
-      </c>
-      <c r="C2" t="s" s="26">
-        <v>45</v>
+      <c r="A2" t="s" s="27">
+        <v>49</v>
+      </c>
+      <c r="B2" t="s" s="28">
+        <v>50</v>
+      </c>
+      <c r="C2" t="s" s="31">
+        <v>53</v>
       </c>
       <c r="D2" s="13" t="s">
         <v>30</v>
@@ -821,7 +860,7 @@
         <v>11</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>46</v>
+        <v>54</v>
       </c>
       <c r="F3" s="13">
         <v>1323</v>
@@ -843,7 +882,7 @@
         <v>12</v>
       </c>
       <c r="E4" s="22" t="s">
-        <v>47</v>
+        <v>55</v>
       </c>
       <c r="F4" s="20">
         <v>1323</v>
@@ -865,7 +904,7 @@
         <v>13</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>48</v>
+        <v>56</v>
       </c>
       <c r="F5" s="20">
         <v>1323</v>

</xml_diff>

<commit_message>
User Already Exists then retry the Process code Updated
</commit_message>
<xml_diff>
--- a/src/test/resources/ExcelFiles/AssessmentCenterDetails.xlsx
+++ b/src/test/resources/ExcelFiles/AssessmentCenterDetails.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="64">
   <si>
     <t>FirstName</t>
   </si>
@@ -193,6 +193,27 @@
   </si>
   <si>
     <t>34255</t>
+  </si>
+  <si>
+    <t>FPK12School27503</t>
+  </si>
+  <si>
+    <t>38144</t>
+  </si>
+  <si>
+    <t>4639</t>
+  </si>
+  <si>
+    <t>81573</t>
+  </si>
+  <si>
+    <t>72242</t>
+  </si>
+  <si>
+    <t>11142</t>
+  </si>
+  <si>
+    <t>39917</t>
   </si>
 </sst>
 </file>
@@ -350,7 +371,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -413,6 +434,9 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyAlignment="true" applyBorder="true">
       <alignment vertical="center" horizontal="center"/>
     </xf>
@@ -809,8 +833,8 @@
       <c r="O1" s="10"/>
     </row>
     <row r="2" spans="1:18" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" t="s" s="27">
-        <v>49</v>
+      <c r="A2" t="s" s="32">
+        <v>57</v>
       </c>
       <c r="B2" t="s" s="28">
         <v>50</v>
@@ -860,7 +884,7 @@
         <v>11</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>54</v>
+        <v>63</v>
       </c>
       <c r="F3" s="13">
         <v>1323</v>
@@ -878,11 +902,9 @@
       <c r="A4" s="6"/>
       <c r="B4" s="6"/>
       <c r="C4" s="6"/>
-      <c r="D4" s="2" t="s">
-        <v>12</v>
-      </c>
+      <c r="D4" s="2"/>
       <c r="E4" s="22" t="s">
-        <v>55</v>
+        <v>34</v>
       </c>
       <c r="F4" s="20">
         <v>1323</v>
@@ -900,11 +922,9 @@
       <c r="A5" s="13"/>
       <c r="B5" s="13"/>
       <c r="C5" s="13"/>
-      <c r="D5" s="2" t="s">
-        <v>13</v>
-      </c>
+      <c r="D5" s="2"/>
       <c r="E5" s="2" t="s">
-        <v>56</v>
+        <v>34</v>
       </c>
       <c r="F5" s="20">
         <v>1323</v>

</xml_diff>

<commit_message>
LMS prod Configuration Setup
</commit_message>
<xml_diff>
--- a/src/test/resources/ExcelFiles/AssessmentCenterDetails.xlsx
+++ b/src/test/resources/ExcelFiles/AssessmentCenterDetails.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Focalpoint Automation\FPK12AutomationProject\src\test\resources\ExcelFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F261F43-511D-4069-9B54-2FC3A12C4EEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CA0E68B-0574-4010-A6D7-5B2E71F4D7CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3240" yWindow="3240" windowWidth="17280" windowHeight="8880" xr2:uid="{27F2060D-2339-4B57-B45F-F65D856F6695}"/>
+    <workbookView xWindow="2688" yWindow="2688" windowWidth="17280" windowHeight="8880" activeTab="1" xr2:uid="{27F2060D-2339-4B57-B45F-F65D856F6695}"/>
   </bookViews>
   <sheets>
     <sheet name="STAGE" sheetId="1" r:id="rId1"/>
+    <sheet name="LMSPROD" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="38">
   <si>
     <t>SchoolName</t>
   </si>
@@ -104,109 +105,52 @@
     <t>Automation Test</t>
   </si>
   <si>
-    <t>FPK12School12601</t>
-  </si>
-  <si>
-    <t>FPK12Classroom64574</t>
-  </si>
-  <si>
-    <t>FPK12Section91315</t>
-  </si>
-  <si>
-    <t>80075</t>
+    <t>FPK12School34026</t>
+  </si>
+  <si>
+    <t>FPK12Classroom22666</t>
+  </si>
+  <si>
+    <t>FPK12Section36695</t>
+  </si>
+  <si>
+    <t>68549</t>
+  </si>
+  <si>
+    <t>47755</t>
+  </si>
+  <si>
+    <t>5008</t>
+  </si>
+  <si>
+    <t>fpadmin</t>
+  </si>
+  <si>
+    <t>qa</t>
+  </si>
+  <si>
+    <t>Mathematics</t>
+  </si>
+  <si>
+    <t>FPK12School67796</t>
+  </si>
+  <si>
+    <t>FPK12Classroom38788</t>
+  </si>
+  <si>
+    <t>FPK12Section70605</t>
+  </si>
+  <si>
+    <t>76623</t>
   </si>
   <si>
     <t>0</t>
   </si>
   <si>
-    <t>68754</t>
-  </si>
-  <si>
-    <t>21896</t>
-  </si>
-  <si>
-    <t>FPK12School72050</t>
-  </si>
-  <si>
-    <t>FPK12Classroom2885</t>
-  </si>
-  <si>
-    <t>FPK12Section90982</t>
-  </si>
-  <si>
-    <t>29484</t>
-  </si>
-  <si>
-    <t>71978</t>
-  </si>
-  <si>
-    <t>45119</t>
-  </si>
-  <si>
-    <t>FPK12School74432</t>
-  </si>
-  <si>
-    <t>FPK12Classroom1531</t>
-  </si>
-  <si>
-    <t>FPK12Section166</t>
-  </si>
-  <si>
-    <t>69421</t>
-  </si>
-  <si>
-    <t>FPK12School37433</t>
-  </si>
-  <si>
-    <t>FPK12Classroom68048</t>
-  </si>
-  <si>
-    <t>FPK12Section32330</t>
-  </si>
-  <si>
-    <t>95173</t>
-  </si>
-  <si>
-    <t>79113</t>
-  </si>
-  <si>
-    <t>33957</t>
-  </si>
-  <si>
-    <t>FPK12School88152</t>
-  </si>
-  <si>
-    <t>FPK12Classroom2919</t>
-  </si>
-  <si>
-    <t>FPK12Section95586</t>
-  </si>
-  <si>
-    <t>31523</t>
-  </si>
-  <si>
-    <t>19229</t>
-  </si>
-  <si>
-    <t>17054</t>
-  </si>
-  <si>
-    <t>FPK12School98467</t>
-  </si>
-  <si>
-    <t>FPK12Classroom30753</t>
-  </si>
-  <si>
-    <t>FPK12Section56147</t>
-  </si>
-  <si>
-    <t>49952</t>
-  </si>
-  <si>
-    <t>93007</t>
-  </si>
-  <si>
-    <t>50315</t>
+    <t>88637</t>
+  </si>
+  <si>
+    <t>FPK12School17155</t>
   </si>
 </sst>
 </file>
@@ -214,7 +158,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="0"/>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -238,6 +182,12 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF1E88E5"/>
+      <name val="Arial"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -281,17 +231,6 @@
     <border>
       <left/>
       <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
         <color indexed="64"/>
       </right>
       <top style="thin">
@@ -299,6 +238,17 @@
       </top>
       <bottom style="thin">
         <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -313,21 +263,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -355,48 +302,10 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyAlignment="true" applyBorder="true">
-      <alignment vertical="center" horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyAlignment="true" applyBorder="true">
-      <alignment vertical="center" horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyAlignment="true" applyBorder="true">
-      <alignment vertical="center" horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyAlignment="true" applyBorder="true">
-      <alignment vertical="center" horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyAlignment="true" applyBorder="true">
-      <alignment vertical="center" horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyAlignment="true" applyBorder="true">
-      <alignment vertical="center" horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyAlignment="true" applyBorder="true">
-      <alignment vertical="center" horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyAlignment="true" applyBorder="true">
-      <alignment vertical="center" horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyAlignment="true" applyBorder="true">
-      <alignment vertical="center" horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyAlignment="true" applyBorder="true">
-      <alignment vertical="center" horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyAlignment="true" applyBorder="true">
-      <alignment vertical="center" horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyAlignment="true" applyBorder="true">
-      <alignment vertical="center" horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyAlignment="true" applyBorder="true">
-      <alignment vertical="center" horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyAlignment="true" applyBorder="true">
-      <alignment vertical="center" horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyAlignment="true" applyBorder="true">
       <alignment vertical="center" horizontal="center"/>
     </xf>
@@ -745,8 +654,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{911B00C3-5650-485D-8FD9-0F4E0599A6CF}">
   <dimension ref="A1:L6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -764,130 +673,281 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="B1" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="C1" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="10" t="s">
+      <c r="D1" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="10" t="s">
+      <c r="E1" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="10" t="s">
+      <c r="F1" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="10" t="s">
+      <c r="G1" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="11" t="s">
+      <c r="H1" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="12" t="s">
+      <c r="I1" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="13" t="s">
+      <c r="J1" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="14" t="s">
+      <c r="K1" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="14" t="s">
+      <c r="L1" s="13" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:12" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" t="s" s="30">
-        <v>51</v>
-      </c>
-      <c r="B2" t="s" s="31">
-        <v>52</v>
-      </c>
-      <c r="C2" t="s" s="32">
-        <v>53</v>
-      </c>
-      <c r="D2" s="3" t="s">
+      <c r="A2" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E2" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="F2" s="4">
+      <c r="F2" s="3">
         <v>1370</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="G2" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="H2" s="5" t="s">
+      <c r="H2" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="I2" s="6">
+      <c r="I2" s="5">
         <v>2024</v>
       </c>
-      <c r="J2" s="6" t="s">
+      <c r="J2" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="K2" s="7" t="s">
+      <c r="K2" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="L2" s="7" t="s">
+      <c r="L2" s="6" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="D3" s="8" t="s">
+      <c r="D3" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="E3" s="8" t="s">
-        <v>54</v>
-      </c>
-      <c r="F3" s="4">
+      <c r="E3" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="F3" s="3">
         <v>1370</v>
       </c>
-      <c r="G3" s="6" t="s">
+      <c r="G3" s="5" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="D4" s="8" t="s">
+      <c r="D4" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="E4" s="8" t="s">
-        <v>55</v>
-      </c>
-      <c r="F4" s="4">
+      <c r="E4" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="F4" s="3">
         <v>1370</v>
       </c>
-      <c r="G4" s="6" t="s">
+      <c r="G4" s="5" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A5" s="9"/>
-      <c r="B5" s="9"/>
-      <c r="C5" s="9"/>
-      <c r="D5" s="8" t="s">
+      <c r="A5" s="8"/>
+      <c r="B5" s="8"/>
+      <c r="C5" s="8"/>
+      <c r="D5" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="E5" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="F5" s="4">
+      <c r="E5" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="F5" s="3">
         <v>1370</v>
       </c>
-      <c r="G5" s="6" t="s">
+      <c r="G5" s="5" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A6" s="9"/>
-      <c r="B6" s="9"/>
-      <c r="C6" s="9"/>
+      <c r="A6" s="8"/>
+      <c r="B6" s="8"/>
+      <c r="C6" s="8"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4110C51E-ADD3-40EA-A3F1-CB649A184727}">
+  <dimension ref="A1:L6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="L2" sqref="L2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" customWidth="true" width="30.0"/>
+    <col min="2" max="2" customWidth="true" width="23.5546875"/>
+    <col min="3" max="3" customWidth="true" width="24.77734375"/>
+    <col min="4" max="4" customWidth="true" style="1" width="19.88671875"/>
+    <col min="5" max="5" customWidth="true" style="1" width="23.77734375"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" style="1" width="20.5546875"/>
+    <col min="8" max="8" customWidth="true" width="31.5546875"/>
+    <col min="10" max="10" customWidth="true" width="19.77734375"/>
+    <col min="11" max="11" customWidth="true" width="15.0"/>
+    <col min="12" max="12" customWidth="true" width="18.33203125"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="13" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" t="s" s="19">
+        <v>37</v>
+      </c>
+      <c r="B2" t="s" s="17">
+        <v>32</v>
+      </c>
+      <c r="C2" t="s" s="18">
+        <v>33</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="F2" s="3">
+        <v>242</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="I2" s="5">
+        <v>2024</v>
+      </c>
+      <c r="J2" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="K2" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="L2" s="15" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="D3" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="F3" s="3">
+        <v>242</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="D4" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="F4" s="3">
+        <v>242</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A5" s="8"/>
+      <c r="B5" s="8"/>
+      <c r="C5" s="8"/>
+      <c r="D5" s="7"/>
+      <c r="E5" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="F5" s="3">
+        <v>242</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A6" s="8"/>
+      <c r="B6" s="8"/>
+      <c r="C6" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
LMS prod Configuration Set Up
</commit_message>
<xml_diff>
--- a/src/test/resources/ExcelFiles/AssessmentCenterDetails.xlsx
+++ b/src/test/resources/ExcelFiles/AssessmentCenterDetails.xlsx
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="49">
   <si>
     <t>SchoolName</t>
   </si>
@@ -151,6 +151,39 @@
   </si>
   <si>
     <t>FPK12School17155</t>
+  </si>
+  <si>
+    <t>FPK12Classroom35333</t>
+  </si>
+  <si>
+    <t>FPK12Section15795</t>
+  </si>
+  <si>
+    <t>30211</t>
+  </si>
+  <si>
+    <t>5587</t>
+  </si>
+  <si>
+    <t>24937</t>
+  </si>
+  <si>
+    <t>FPK12School95878</t>
+  </si>
+  <si>
+    <t>FPK12Classroom27824</t>
+  </si>
+  <si>
+    <t>FPK12Section13722</t>
+  </si>
+  <si>
+    <t>43388</t>
+  </si>
+  <si>
+    <t>9801</t>
+  </si>
+  <si>
+    <t>38240</t>
   </si>
 </sst>
 </file>
@@ -263,7 +296,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -306,6 +339,21 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyAlignment="true" applyBorder="true">
       <alignment vertical="center" horizontal="center"/>
     </xf>
@@ -864,14 +912,14 @@
       </c>
     </row>
     <row r="2" spans="1:12" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" t="s" s="19">
-        <v>37</v>
-      </c>
-      <c r="B2" t="s" s="17">
-        <v>32</v>
-      </c>
-      <c r="C2" t="s" s="18">
-        <v>33</v>
+      <c r="A2" t="s" s="22">
+        <v>43</v>
+      </c>
+      <c r="B2" t="s" s="23">
+        <v>44</v>
+      </c>
+      <c r="C2" t="s" s="24">
+        <v>45</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>28</v>
@@ -906,7 +954,7 @@
         <v>18</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>34</v>
+        <v>46</v>
       </c>
       <c r="F3" s="3">
         <v>242</v>
@@ -920,7 +968,7 @@
         <v>19</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>36</v>
+        <v>47</v>
       </c>
       <c r="F4" s="3">
         <v>242</v>
@@ -933,9 +981,11 @@
       <c r="A5" s="8"/>
       <c r="B5" s="8"/>
       <c r="C5" s="8"/>
-      <c r="D5" s="7"/>
+      <c r="D5" s="7" t="s">
+        <v>20</v>
+      </c>
       <c r="E5" s="7" t="s">
-        <v>35</v>
+        <v>48</v>
       </c>
       <c r="F5" s="3">
         <v>242</v>

</xml_diff>

<commit_message>
LMS Prod Setup Config
</commit_message>
<xml_diff>
--- a/src/test/resources/ExcelFiles/AssessmentCenterDetails.xlsx
+++ b/src/test/resources/ExcelFiles/AssessmentCenterDetails.xlsx
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="55">
   <si>
     <t>SchoolName</t>
   </si>
@@ -184,6 +184,24 @@
   </si>
   <si>
     <t>38240</t>
+  </si>
+  <si>
+    <t>FPK12School26427</t>
+  </si>
+  <si>
+    <t>FPK12School42740</t>
+  </si>
+  <si>
+    <t>FPK12School22131</t>
+  </si>
+  <si>
+    <t>FPK12School72875</t>
+  </si>
+  <si>
+    <t>FPK12Classroom50751</t>
+  </si>
+  <si>
+    <t>FPK12Section65933</t>
   </si>
 </sst>
 </file>
@@ -296,7 +314,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -339,6 +357,24 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyAlignment="true" applyBorder="true">
       <alignment vertical="center" horizontal="center"/>
     </xf>
@@ -912,14 +948,14 @@
       </c>
     </row>
     <row r="2" spans="1:12" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" t="s" s="22">
-        <v>43</v>
-      </c>
-      <c r="B2" t="s" s="23">
-        <v>44</v>
-      </c>
-      <c r="C2" t="s" s="24">
-        <v>45</v>
+      <c r="A2" t="s" s="28">
+        <v>52</v>
+      </c>
+      <c r="B2" t="s" s="29">
+        <v>53</v>
+      </c>
+      <c r="C2" t="s" s="30">
+        <v>54</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>28</v>

</xml_diff>

<commit_message>
Latest Script and Updated Standards Selection Logic
</commit_message>
<xml_diff>
--- a/src/test/resources/ExcelFiles/AssessmentCenterDetails.xlsx
+++ b/src/test/resources/ExcelFiles/AssessmentCenterDetails.xlsx
@@ -3,14 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr defaultThemeVersion="202300"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Focalpoint Automation\FPK12AutomationProject\src\test\resources\ExcelFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CA0E68B-0574-4010-A6D7-5B2E71F4D7CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3B2D03B-3CBE-4EA2-AEAF-FB9D0FBD2322}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2688" yWindow="2688" windowWidth="17280" windowHeight="8880" activeTab="1" xr2:uid="{27F2060D-2339-4B57-B45F-F65D856F6695}"/>
+    <workbookView xWindow="3036" yWindow="3036" windowWidth="17280" windowHeight="8880" xr2:uid="{27F2060D-2339-4B57-B45F-F65D856F6695}"/>
   </bookViews>
   <sheets>
     <sheet name="STAGE" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="37">
   <si>
     <t>SchoolName</t>
   </si>
@@ -75,9 +75,6 @@
     <t>Subject</t>
   </si>
   <si>
-    <t>fpk12district</t>
-  </si>
-  <si>
     <t>user</t>
   </si>
   <si>
@@ -132,84 +129,32 @@
     <t>Mathematics</t>
   </si>
   <si>
-    <t>FPK12School67796</t>
-  </si>
-  <si>
-    <t>FPK12Classroom38788</t>
-  </si>
-  <si>
-    <t>FPK12Section70605</t>
-  </si>
-  <si>
-    <t>76623</t>
-  </si>
-  <si>
-    <t>0</t>
-  </si>
-  <si>
-    <t>88637</t>
-  </si>
-  <si>
-    <t>FPK12School17155</t>
-  </si>
-  <si>
-    <t>FPK12Classroom35333</t>
-  </si>
-  <si>
-    <t>FPK12Section15795</t>
-  </si>
-  <si>
-    <t>30211</t>
-  </si>
-  <si>
-    <t>5587</t>
-  </si>
-  <si>
-    <t>24937</t>
-  </si>
-  <si>
-    <t>FPK12School95878</t>
-  </si>
-  <si>
-    <t>FPK12Classroom27824</t>
-  </si>
-  <si>
-    <t>FPK12Section13722</t>
-  </si>
-  <si>
-    <t>43388</t>
-  </si>
-  <si>
-    <t>9801</t>
-  </si>
-  <si>
-    <t>38240</t>
-  </si>
-  <si>
-    <t>FPK12School26427</t>
-  </si>
-  <si>
-    <t>FPK12School42740</t>
-  </si>
-  <si>
-    <t>FPK12School22131</t>
-  </si>
-  <si>
-    <t>FPK12School72875</t>
-  </si>
-  <si>
-    <t>FPK12Classroom50751</t>
-  </si>
-  <si>
-    <t>FPK12Section65933</t>
+    <t>FPK12School22538</t>
+  </si>
+  <si>
+    <t>FPK12Classroom3592</t>
+  </si>
+  <si>
+    <t>FPK12Section67301</t>
+  </si>
+  <si>
+    <t>57896</t>
+  </si>
+  <si>
+    <t>14780</t>
+  </si>
+  <si>
+    <t>53513</t>
+  </si>
+  <si>
+    <t>fpdistrict</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -241,6 +186,13 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="8"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -256,7 +208,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -304,17 +256,21 @@
       <diagonal/>
     </border>
     <border>
-      <bottom style="thin"/>
-    </border>
-    <border>
-      <right style="thin"/>
-      <bottom style="thin"/>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -357,51 +313,10 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyAlignment="true" applyBorder="true">
-      <alignment vertical="center" horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyAlignment="true" applyBorder="true">
-      <alignment vertical="center" horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyAlignment="true" applyBorder="true">
-      <alignment vertical="center" horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyAlignment="true" applyBorder="true">
-      <alignment vertical="center" horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyAlignment="true" applyBorder="true">
-      <alignment vertical="center" horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyAlignment="true" applyBorder="true">
-      <alignment vertical="center" horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyAlignment="true" applyBorder="true">
-      <alignment vertical="center" horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyAlignment="true" applyBorder="true">
-      <alignment vertical="center" horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyAlignment="true" applyBorder="true">
-      <alignment vertical="center" horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyAlignment="true" applyBorder="true">
-      <alignment vertical="center" horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyAlignment="true" applyBorder="true">
-      <alignment vertical="center" horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyAlignment="true" applyBorder="true">
-      <alignment vertical="center" horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyAlignment="true" applyBorder="true">
-      <alignment vertical="center" horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyAlignment="true" applyBorder="true">
-      <alignment vertical="center" horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyAlignment="true" applyBorder="true">
-      <alignment vertical="center" horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -738,22 +653,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{911B00C3-5650-485D-8FD9-0F4E0599A6CF}">
   <dimension ref="A1:L6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="30.0"/>
-    <col min="2" max="2" customWidth="true" width="23.5546875"/>
-    <col min="3" max="3" customWidth="true" width="24.77734375"/>
-    <col min="4" max="4" customWidth="true" style="1" width="19.88671875"/>
-    <col min="5" max="5" customWidth="true" style="1" width="23.77734375"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" style="1" width="20.5546875"/>
-    <col min="8" max="8" customWidth="true" width="31.5546875"/>
-    <col min="10" max="10" customWidth="true" width="19.77734375"/>
-    <col min="11" max="11" customWidth="true" width="15.0"/>
-    <col min="12" max="12" customWidth="true" width="18.33203125"/>
+    <col min="1" max="1" width="30" customWidth="1"/>
+    <col min="2" max="2" width="23.5546875" customWidth="1"/>
+    <col min="3" max="3" width="24.77734375" customWidth="1"/>
+    <col min="4" max="4" width="19.88671875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="23.77734375" style="1" customWidth="1"/>
+    <col min="7" max="7" width="20.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="31.5546875" customWidth="1"/>
+    <col min="10" max="10" width="19.77734375" customWidth="1"/>
+    <col min="11" max="11" width="15" customWidth="1"/>
+    <col min="12" max="12" width="18.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
@@ -796,68 +711,68 @@
     </row>
     <row r="2" spans="1:12" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="B2" s="14" t="s">
+      <c r="C2" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="C2" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="E2" s="3" t="s">
         <v>12</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>13</v>
       </c>
       <c r="F2" s="3">
         <v>1370</v>
       </c>
       <c r="G2" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="H2" s="4" t="s">
         <v>14</v>
-      </c>
-      <c r="H2" s="4" t="s">
-        <v>15</v>
       </c>
       <c r="I2" s="5">
         <v>2024</v>
       </c>
       <c r="J2" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="K2" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="L2" s="6" t="s">
         <v>16</v>
-      </c>
-      <c r="L2" s="6" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="D3" s="7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F3" s="3">
         <v>1370</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="D4" s="7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F4" s="3">
         <v>1370</v>
       </c>
       <c r="G4" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.3">
@@ -865,16 +780,16 @@
       <c r="B5" s="8"/>
       <c r="C5" s="8"/>
       <c r="D5" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F5" s="3">
         <v>1370</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.3">
@@ -891,22 +806,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4110C51E-ADD3-40EA-A3F1-CB649A184727}">
   <dimension ref="A1:L6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="30.0"/>
-    <col min="2" max="2" customWidth="true" width="23.5546875"/>
-    <col min="3" max="3" customWidth="true" width="24.77734375"/>
-    <col min="4" max="4" customWidth="true" style="1" width="19.88671875"/>
-    <col min="5" max="5" customWidth="true" style="1" width="23.77734375"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" style="1" width="20.5546875"/>
-    <col min="8" max="8" customWidth="true" width="31.5546875"/>
-    <col min="10" max="10" customWidth="true" width="19.77734375"/>
-    <col min="11" max="11" customWidth="true" width="15.0"/>
-    <col min="12" max="12" customWidth="true" width="18.33203125"/>
+    <col min="1" max="1" width="30" customWidth="1"/>
+    <col min="2" max="2" width="23.5546875" customWidth="1"/>
+    <col min="3" max="3" width="24.77734375" customWidth="1"/>
+    <col min="4" max="4" width="19.88671875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="23.77734375" style="1" customWidth="1"/>
+    <col min="7" max="7" width="20.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="31.5546875" customWidth="1"/>
+    <col min="10" max="10" width="19.77734375" customWidth="1"/>
+    <col min="11" max="11" width="15" customWidth="1"/>
+    <col min="12" max="12" width="18.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
@@ -948,69 +863,69 @@
       </c>
     </row>
     <row r="2" spans="1:12" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" t="s" s="28">
-        <v>52</v>
-      </c>
-      <c r="B2" t="s" s="29">
-        <v>53</v>
-      </c>
-      <c r="C2" t="s" s="30">
-        <v>54</v>
+      <c r="A2" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="B2" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="C2" s="16" t="s">
+        <v>32</v>
       </c>
       <c r="D2" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E2" s="3" t="s">
         <v>28</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>29</v>
       </c>
       <c r="F2" s="3">
         <v>242</v>
       </c>
       <c r="G2" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="H2" s="4" t="s">
         <v>14</v>
-      </c>
-      <c r="H2" s="4" t="s">
-        <v>15</v>
       </c>
       <c r="I2" s="5">
         <v>2024</v>
       </c>
       <c r="J2" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="K2" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="L2" s="15" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="D3" s="7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>46</v>
+        <v>33</v>
       </c>
       <c r="F3" s="3">
         <v>242</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="D4" s="7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>47</v>
+        <v>34</v>
       </c>
       <c r="F4" s="3">
         <v>242</v>
       </c>
       <c r="G4" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.3">
@@ -1018,16 +933,16 @@
       <c r="B5" s="8"/>
       <c r="C5" s="8"/>
       <c r="D5" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>48</v>
+        <v>35</v>
       </c>
       <c r="F5" s="3">
         <v>242</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Latest Script and Enhancing the Script for Concern Screen
</commit_message>
<xml_diff>
--- a/src/test/resources/ExcelFiles/AssessmentCenterDetails.xlsx
+++ b/src/test/resources/ExcelFiles/AssessmentCenterDetails.xlsx
@@ -3,14 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr defaultThemeVersion="202300"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Focalpoint Automation\FPK12AutomationProject\src\test\resources\ExcelFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3B2D03B-3CBE-4EA2-AEAF-FB9D0FBD2322}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F01EB14-7050-4A4D-A158-C63C8263516E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3036" yWindow="3036" windowWidth="17280" windowHeight="8880" xr2:uid="{27F2060D-2339-4B57-B45F-F65D856F6695}"/>
+    <workbookView xWindow="3036" yWindow="3036" windowWidth="17280" windowHeight="8880" activeTab="1" xr2:uid="{27F2060D-2339-4B57-B45F-F65D856F6695}"/>
   </bookViews>
   <sheets>
     <sheet name="STAGE" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="53">
   <si>
     <t>SchoolName</t>
   </si>
@@ -129,31 +129,80 @@
     <t>Mathematics</t>
   </si>
   <si>
-    <t>FPK12School22538</t>
-  </si>
-  <si>
-    <t>FPK12Classroom3592</t>
-  </si>
-  <si>
-    <t>FPK12Section67301</t>
-  </si>
-  <si>
-    <t>57896</t>
-  </si>
-  <si>
-    <t>14780</t>
-  </si>
-  <si>
-    <t>53513</t>
-  </si>
-  <si>
     <t>fpdistrict</t>
+  </si>
+  <si>
+    <t>FPK12School22646</t>
+  </si>
+  <si>
+    <t>FPK12Classroom56973</t>
+  </si>
+  <si>
+    <t>FPK12Section78958</t>
+  </si>
+  <si>
+    <t>36393</t>
+  </si>
+  <si>
+    <t>42259</t>
+  </si>
+  <si>
+    <t>7643</t>
+  </si>
+  <si>
+    <t>FPK12School4857</t>
+  </si>
+  <si>
+    <t>FPK12Classroom17154</t>
+  </si>
+  <si>
+    <t>FPK12Section19193</t>
+  </si>
+  <si>
+    <t>FPK12School82559</t>
+  </si>
+  <si>
+    <t>FPK12Classroom18397</t>
+  </si>
+  <si>
+    <t>FPK12Section62383</t>
+  </si>
+  <si>
+    <t>72728</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>99661</t>
+  </si>
+  <si>
+    <t>95152</t>
+  </si>
+  <si>
+    <t>FPK12School71871</t>
+  </si>
+  <si>
+    <t>FPK12Classroom77158</t>
+  </si>
+  <si>
+    <t>FPK12Section13169</t>
+  </si>
+  <si>
+    <t>96441</t>
+  </si>
+  <si>
+    <t>35549</t>
+  </si>
+  <si>
+    <t>77223</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -208,7 +257,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -266,11 +315,18 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <right style="thin"/>
+      <bottom style="thin"/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -313,10 +369,37 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -653,22 +736,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{911B00C3-5650-485D-8FD9-0F4E0599A6CF}">
   <dimension ref="A1:L6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="30" customWidth="1"/>
-    <col min="2" max="2" width="23.5546875" customWidth="1"/>
-    <col min="3" max="3" width="24.77734375" customWidth="1"/>
-    <col min="4" max="4" width="19.88671875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="23.77734375" style="1" customWidth="1"/>
-    <col min="7" max="7" width="20.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="31.5546875" customWidth="1"/>
-    <col min="10" max="10" width="19.77734375" customWidth="1"/>
-    <col min="11" max="11" width="15" customWidth="1"/>
-    <col min="12" max="12" width="18.33203125" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="30.0"/>
+    <col min="2" max="2" customWidth="true" width="23.5546875"/>
+    <col min="3" max="3" customWidth="true" width="24.77734375"/>
+    <col min="4" max="4" customWidth="true" style="1" width="19.88671875"/>
+    <col min="5" max="5" customWidth="true" style="1" width="23.77734375"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" style="1" width="20.5546875"/>
+    <col min="8" max="8" customWidth="true" width="31.5546875"/>
+    <col min="10" max="10" customWidth="true" width="19.77734375"/>
+    <col min="11" max="11" customWidth="true" width="15.0"/>
+    <col min="12" max="12" customWidth="true" width="18.33203125"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
@@ -710,17 +793,17 @@
       </c>
     </row>
     <row r="2" spans="1:12" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="B2" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="C2" s="14" t="s">
-        <v>23</v>
-      </c>
-      <c r="D2" s="17" t="s">
-        <v>36</v>
+      <c r="A2" t="s" s="24">
+        <v>47</v>
+      </c>
+      <c r="B2" t="s" s="25">
+        <v>48</v>
+      </c>
+      <c r="C2" t="s" s="26">
+        <v>49</v>
+      </c>
+      <c r="D2" s="16" t="s">
+        <v>30</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>12</v>
@@ -752,7 +835,7 @@
         <v>17</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>24</v>
+        <v>50</v>
       </c>
       <c r="F3" s="3">
         <v>1370</v>
@@ -766,7 +849,7 @@
         <v>18</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>25</v>
+        <v>51</v>
       </c>
       <c r="F4" s="3">
         <v>1370</v>
@@ -783,7 +866,7 @@
         <v>19</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>26</v>
+        <v>52</v>
       </c>
       <c r="F5" s="3">
         <v>1370</v>
@@ -806,22 +889,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4110C51E-ADD3-40EA-A3F1-CB649A184727}">
   <dimension ref="A1:L6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L2" sqref="L2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="30" customWidth="1"/>
-    <col min="2" max="2" width="23.5546875" customWidth="1"/>
-    <col min="3" max="3" width="24.77734375" customWidth="1"/>
-    <col min="4" max="4" width="19.88671875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="23.77734375" style="1" customWidth="1"/>
-    <col min="7" max="7" width="20.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="31.5546875" customWidth="1"/>
-    <col min="10" max="10" width="19.77734375" customWidth="1"/>
-    <col min="11" max="11" width="15" customWidth="1"/>
-    <col min="12" max="12" width="18.33203125" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="30.0"/>
+    <col min="2" max="2" customWidth="true" width="23.5546875"/>
+    <col min="3" max="3" customWidth="true" width="24.77734375"/>
+    <col min="4" max="4" customWidth="true" style="1" width="19.88671875"/>
+    <col min="5" max="5" customWidth="true" style="1" width="23.77734375"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" style="1" width="20.5546875"/>
+    <col min="8" max="8" customWidth="true" width="31.5546875"/>
+    <col min="10" max="10" customWidth="true" width="19.77734375"/>
+    <col min="11" max="11" customWidth="true" width="15.0"/>
+    <col min="12" max="12" customWidth="true" width="18.33203125"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
@@ -863,14 +946,14 @@
       </c>
     </row>
     <row r="2" spans="1:12" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="16" t="s">
-        <v>30</v>
-      </c>
-      <c r="B2" s="16" t="s">
+      <c r="A2" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="C2" s="16" t="s">
+      <c r="B2" s="17" t="s">
         <v>32</v>
+      </c>
+      <c r="C2" s="17" t="s">
+        <v>33</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>27</v>
@@ -905,7 +988,7 @@
         <v>17</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F3" s="3">
         <v>242</v>
@@ -919,7 +1002,7 @@
         <v>18</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="F4" s="3">
         <v>242</v>
@@ -936,7 +1019,7 @@
         <v>19</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="F5" s="3">
         <v>242</v>

</xml_diff>